<commit_message>
Update and add exported versions of drawio files
</commit_message>
<xml_diff>
--- a/Cronograma - SITUA.xlsx
+++ b/Cronograma - SITUA.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>Parte</t>
   </si>
@@ -64,7 +64,7 @@
     <t>Baixa</t>
   </si>
   <si>
-    <t>Ambiente</t>
+    <t>Ambiente, Estético, etc.</t>
   </si>
   <si>
     <t>Interface de usuário</t>
@@ -79,7 +79,7 @@
     <t>Protótipo</t>
   </si>
   <si>
-    <t>Documentação</t>
+    <t>Melhorias e Documentação</t>
   </si>
   <si>
     <t>Sensores</t>
@@ -91,7 +91,10 @@
     <t>Semáforo inteligente</t>
   </si>
   <si>
-    <t>Indicador de trânsito a frente</t>
+    <t>Placa de sinalização de trânsito</t>
+  </si>
+  <si>
+    <t>Implementação</t>
   </si>
 </sst>
 </file>
@@ -293,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -334,16 +337,22 @@
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
@@ -741,15 +750,13 @@
       <c r="G4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="7" t="s">
+      <c r="H4" s="7"/>
+      <c r="J4" s="14" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="10" t="s">
@@ -760,17 +767,17 @@
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
     </row>
     <row r="6">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="17" t="s">
         <v>25</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -791,28 +798,26 @@
       <c r="J6" s="7"/>
     </row>
     <row r="7">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="18" t="b">
+      <c r="C7" s="20" t="b">
         <v>0</v>
       </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="20" t="s">
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="19"/>
-      <c r="H7" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" s="20"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
     </row>
   </sheetData>
   <dataValidations>

</xml_diff>